<commit_message>
add new methods to handle order
</commit_message>
<xml_diff>
--- a/source/happy.cd.design.xlsx
+++ b/source/happy.cd.design.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="18195" windowHeight="7380" tabRatio="889" firstSheet="4" activeTab="11"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="490">
   <si>
     <t>Google PR</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -214,7 +214,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -232,7 +232,7 @@
         <b/>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -243,7 +243,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -255,7 +255,7 @@
         <b/>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -266,7 +266,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -653,7 +653,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -989,7 +989,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1382,7 +1382,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1393,7 +1393,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1423,7 +1423,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1434,7 +1434,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1480,7 +1480,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1491,7 +1491,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1503,7 +1503,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1514,7 +1514,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1526,7 +1526,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1537,7 +1537,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1583,7 +1583,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1594,7 +1594,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1612,7 +1612,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1623,7 +1623,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2120,16 +2120,34 @@
     <t>face</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>英语组合</t>
+  </si>
+  <si>
+    <t>ican</t>
+  </si>
+  <si>
+    <t>meili</t>
+  </si>
+  <si>
+    <t>xiyi</t>
+  </si>
+  <si>
+    <t>soso</t>
+  </si>
+  <si>
+    <t>take</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2138,7 +2156,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2146,14 +2164,14 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2161,7 +2179,7 @@
     <font>
       <sz val="16"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2169,7 +2187,7 @@
     <font>
       <sz val="12"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2178,7 +2196,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2186,7 +2204,7 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2195,7 +2213,7 @@
       <b/>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2204,7 +2222,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2213,7 +2231,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2221,7 +2239,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2229,7 +2247,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2237,7 +2255,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2245,14 +2263,14 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2284,7 +2302,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2319,7 +2337,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2335,7 +2353,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2352,6 +2370,14 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -2432,7 +2458,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -2652,17 +2678,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2674,7 +2689,7 @@
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3017,10 +3032,16 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -8949,19 +8970,19 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="12.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="12.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="1"/>
-    <col min="9" max="9" width="12.875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:9" ht="20.25" customHeight="1">
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>0</v>
@@ -8985,7 +9006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:9" ht="20.25" hidden="1" customHeight="1">
       <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
@@ -9011,7 +9032,7 @@
         <v>10600</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:9" ht="20.25" hidden="1" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
@@ -9037,7 +9058,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:9" ht="20.25" hidden="1" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
@@ -9063,7 +9084,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:9" ht="20.25" hidden="1" customHeight="1">
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
@@ -9089,7 +9110,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:9" ht="20.25" customHeight="1">
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
@@ -9115,7 +9136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:9" ht="20.25" customHeight="1">
       <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
@@ -9141,7 +9162,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:9" ht="20.25" customHeight="1">
       <c r="B10" s="4" t="s">
         <v>203</v>
       </c>
@@ -9167,7 +9188,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:9" ht="20.25" customHeight="1">
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
@@ -9193,7 +9214,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:9" ht="20.25" customHeight="1">
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
@@ -9219,7 +9240,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:9" ht="20.25" customHeight="1">
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
@@ -9245,7 +9266,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:9" ht="20.25" customHeight="1">
       <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
@@ -9271,7 +9292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:9" ht="20.25" customHeight="1">
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
@@ -9297,7 +9318,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:9" ht="20.25" customHeight="1">
       <c r="B16" s="4" t="s">
         <v>10</v>
       </c>
@@ -9323,7 +9344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:9" ht="20.25" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
@@ -9349,7 +9370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:9" ht="20.25" customHeight="1">
       <c r="B18" s="5" t="s">
         <v>7</v>
       </c>
@@ -9375,7 +9396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:9" ht="20.25" customHeight="1">
       <c r="B19" s="4" t="s">
         <v>13</v>
       </c>
@@ -9401,7 +9422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:9" ht="20.25" customHeight="1">
       <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
@@ -9423,7 +9444,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:9" ht="20.25" customHeight="1">
       <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
@@ -9445,70 +9466,70 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:9" ht="20.25" customHeight="1">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:9" ht="20.25" customHeight="1">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:9" ht="20.25" customHeight="1">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:9" ht="20.25" customHeight="1">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:9" ht="20.25" customHeight="1">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:9" ht="20.25" customHeight="1">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:9" ht="20.25" customHeight="1">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:9" ht="20.25" customHeight="1">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:9" ht="20.25" customHeight="1">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:9" ht="20.25" customHeight="1">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -9539,17 +9560,17 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="19.5" customHeight="1"/>
   <cols>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="33.625" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" customWidth="1"/>
     <col min="6" max="7" width="29" customWidth="1"/>
-    <col min="8" max="8" width="19.375" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:9" ht="19.5" customHeight="1">
       <c r="B3" s="57" t="s">
         <v>176</v>
       </c>
@@ -9575,7 +9596,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:9" ht="19.5" customHeight="1">
       <c r="C4" s="56" t="s">
         <v>150</v>
       </c>
@@ -9592,7 +9613,7 @@
         <v>16676</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:9" ht="57.75" customHeight="1">
       <c r="C5" s="56" t="s">
         <v>153</v>
       </c>
@@ -9609,7 +9630,7 @@
       <c r="H5" s="56"/>
       <c r="I5" s="56"/>
     </row>
-    <row r="6" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:9" ht="19.5" customHeight="1">
       <c r="C6" s="56" t="s">
         <v>159</v>
       </c>
@@ -9626,7 +9647,7 @@
       <c r="H6" s="56"/>
       <c r="I6" s="56"/>
     </row>
-    <row r="7" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:9" ht="19.5" customHeight="1">
       <c r="B7" s="56"/>
       <c r="C7" s="56" t="s">
         <v>163</v>
@@ -9642,7 +9663,7 @@
       <c r="H7" s="56"/>
       <c r="I7" s="56"/>
     </row>
-    <row r="8" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:9" ht="19.5" customHeight="1">
       <c r="B8" s="56"/>
       <c r="C8" s="56" t="s">
         <v>165</v>
@@ -9658,7 +9679,7 @@
       <c r="H8" s="56"/>
       <c r="I8" s="56"/>
     </row>
-    <row r="9" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:9" ht="19.5" customHeight="1">
       <c r="B9" s="56"/>
       <c r="C9" s="56"/>
       <c r="D9" s="56"/>
@@ -9668,7 +9689,7 @@
       <c r="H9" s="56"/>
       <c r="I9" s="56"/>
     </row>
-    <row r="10" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:9" ht="19.5" customHeight="1">
       <c r="B10" s="56"/>
       <c r="C10" s="56" t="s">
         <v>167</v>
@@ -9684,7 +9705,7 @@
       <c r="H10" s="56"/>
       <c r="I10" s="56"/>
     </row>
-    <row r="11" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:9" ht="19.5" customHeight="1">
       <c r="B11" s="56"/>
       <c r="C11" s="56"/>
       <c r="D11" s="56"/>
@@ -9694,7 +9715,7 @@
       <c r="H11" s="56"/>
       <c r="I11" s="56"/>
     </row>
-    <row r="12" spans="2:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:9" ht="46.5" customHeight="1">
       <c r="B12" s="56"/>
       <c r="C12" s="56" t="s">
         <v>170</v>
@@ -9714,14 +9735,14 @@
       <c r="H12" s="56"/>
       <c r="I12" s="56"/>
     </row>
-    <row r="13" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:9" ht="28.5" customHeight="1">
       <c r="B13" s="56"/>
       <c r="F13" s="56"/>
       <c r="G13" s="56"/>
       <c r="H13" s="56"/>
       <c r="I13" s="56"/>
     </row>
-    <row r="14" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:9" ht="19.5" customHeight="1">
       <c r="B14" s="57" t="s">
         <v>177</v>
       </c>
@@ -9745,7 +9766,7 @@
       </c>
       <c r="I14" s="56"/>
     </row>
-    <row r="15" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:9" ht="19.5" customHeight="1">
       <c r="B15" s="56"/>
       <c r="C15" s="56" t="s">
         <v>175</v>
@@ -9763,7 +9784,7 @@
       <c r="H15" s="56"/>
       <c r="I15" s="56"/>
     </row>
-    <row r="16" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:9" ht="19.5" customHeight="1">
       <c r="B16" s="56"/>
       <c r="C16" s="56"/>
       <c r="D16" s="56"/>
@@ -9773,7 +9794,7 @@
       <c r="H16" s="56"/>
       <c r="I16" s="56"/>
     </row>
-    <row r="17" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:9" ht="19.5" customHeight="1">
       <c r="B17" s="56"/>
       <c r="C17" s="56"/>
       <c r="D17" s="56"/>
@@ -9783,7 +9804,7 @@
       <c r="H17" s="56"/>
       <c r="I17" s="56"/>
     </row>
-    <row r="18" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:9" ht="19.5" customHeight="1">
       <c r="B18" s="56"/>
       <c r="C18" s="56"/>
       <c r="D18" s="56"/>
@@ -9793,7 +9814,7 @@
       <c r="H18" s="56"/>
       <c r="I18" s="56"/>
     </row>
-    <row r="19" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:9" ht="19.5" customHeight="1">
       <c r="B19" s="56" t="s">
         <v>233</v>
       </c>
@@ -9805,7 +9826,7 @@
       <c r="H19" s="56"/>
       <c r="I19" s="56"/>
     </row>
-    <row r="20" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:9" ht="19.5" customHeight="1">
       <c r="B20" s="56"/>
       <c r="C20" s="56"/>
       <c r="D20" s="56" t="s">
@@ -9819,7 +9840,7 @@
       <c r="H20" s="56"/>
       <c r="I20" s="56"/>
     </row>
-    <row r="21" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:9" ht="19.5" customHeight="1">
       <c r="B21" s="56"/>
       <c r="C21" s="56"/>
       <c r="D21" s="56" t="s">
@@ -9833,7 +9854,7 @@
       <c r="H21" s="56"/>
       <c r="I21" s="56"/>
     </row>
-    <row r="22" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:9" ht="19.5" customHeight="1">
       <c r="C22" s="56"/>
       <c r="D22" s="56"/>
       <c r="E22" s="56"/>
@@ -9842,7 +9863,7 @@
       <c r="H22" s="56"/>
       <c r="I22" s="56"/>
     </row>
-    <row r="23" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:9" ht="19.5" customHeight="1">
       <c r="C23" s="56"/>
       <c r="D23" s="56"/>
       <c r="E23" s="56"/>
@@ -9851,7 +9872,7 @@
       <c r="H23" s="56"/>
       <c r="I23" s="56"/>
     </row>
-    <row r="24" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:9" ht="19.5" customHeight="1">
       <c r="C24" s="56"/>
       <c r="D24" s="56"/>
       <c r="E24" s="56"/>
@@ -9886,15 +9907,15 @@
       <selection activeCell="AO25" sqref="AO25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="47" width="2.75" style="7"/>
-    <col min="48" max="48" width="14.375" style="7" customWidth="1"/>
-    <col min="49" max="16384" width="2.75" style="7"/>
+    <col min="1" max="47" width="2.7109375" style="7"/>
+    <col min="48" max="48" width="14.42578125" style="7" customWidth="1"/>
+    <col min="49" max="16384" width="2.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="14:74" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="1" spans="14:74" ht="15.75" thickBot="1"/>
+    <row r="2" spans="14:74">
       <c r="N2" s="8"/>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
@@ -9952,7 +9973,7 @@
       <c r="BP2" s="9"/>
       <c r="BQ2" s="10"/>
     </row>
-    <row r="3" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="3" spans="14:74">
       <c r="N3" s="11"/>
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
@@ -10012,7 +10033,7 @@
       <c r="BP3" s="12"/>
       <c r="BQ3" s="13"/>
     </row>
-    <row r="4" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="4" spans="14:74">
       <c r="N4" s="11"/>
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
@@ -10072,7 +10093,7 @@
       <c r="BP4" s="12"/>
       <c r="BQ4" s="13"/>
     </row>
-    <row r="5" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="5" spans="14:74">
       <c r="N5" s="11"/>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
@@ -10130,7 +10151,7 @@
       <c r="BP5" s="12"/>
       <c r="BQ5" s="13"/>
     </row>
-    <row r="6" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="6" spans="14:74">
       <c r="N6" s="11"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
@@ -10188,7 +10209,7 @@
       <c r="BP6" s="12"/>
       <c r="BQ6" s="13"/>
     </row>
-    <row r="7" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="7" spans="14:74">
       <c r="N7" s="11"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
@@ -10246,7 +10267,7 @@
       <c r="BP7" s="12"/>
       <c r="BQ7" s="13"/>
     </row>
-    <row r="8" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="8" spans="14:74">
       <c r="N8" s="11"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
@@ -10306,7 +10327,7 @@
       <c r="BO8" s="12"/>
       <c r="BR8" s="12"/>
     </row>
-    <row r="9" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="9" spans="14:74">
       <c r="N9" s="11"/>
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
@@ -10363,7 +10384,7 @@
       <c r="BO9" s="12"/>
       <c r="BR9" s="12"/>
     </row>
-    <row r="10" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="10" spans="14:74">
       <c r="N10" s="11"/>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
@@ -10421,7 +10442,7 @@
       <c r="BP10" s="12"/>
       <c r="BQ10" s="13"/>
     </row>
-    <row r="11" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="11" spans="14:74">
       <c r="N11" s="11"/>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
@@ -10483,7 +10504,7 @@
       <c r="BP11" s="12"/>
       <c r="BQ11" s="13"/>
     </row>
-    <row r="12" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="12" spans="14:74">
       <c r="N12" s="11"/>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
@@ -10548,7 +10569,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="13" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="13" spans="14:74">
       <c r="N13" s="11"/>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
@@ -10609,7 +10630,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="14" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="14" spans="14:74">
       <c r="N14" s="11"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
@@ -10670,7 +10691,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="15" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="15" spans="14:74">
       <c r="N15" s="11"/>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
@@ -10731,7 +10752,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="16" spans="14:74" x14ac:dyDescent="0.15">
+    <row r="16" spans="14:74">
       <c r="N16" s="11"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
@@ -10792,7 +10813,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="17" spans="14:69">
       <c r="N17" s="11"/>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
@@ -10850,7 +10871,7 @@
       <c r="BP17" s="12"/>
       <c r="BQ17" s="13"/>
     </row>
-    <row r="18" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="18" spans="14:69">
       <c r="N18" s="11"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
@@ -10908,7 +10929,7 @@
       <c r="BP18" s="12"/>
       <c r="BQ18" s="13"/>
     </row>
-    <row r="19" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="19" spans="14:69">
       <c r="N19" s="11"/>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
@@ -10966,7 +10987,7 @@
       <c r="BP19" s="12"/>
       <c r="BQ19" s="13"/>
     </row>
-    <row r="20" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="20" spans="14:69">
       <c r="N20" s="11"/>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
@@ -11024,7 +11045,7 @@
       <c r="BP20" s="12"/>
       <c r="BQ20" s="13"/>
     </row>
-    <row r="21" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="21" spans="14:69">
       <c r="N21" s="11"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
@@ -11082,7 +11103,7 @@
       <c r="BP21" s="12"/>
       <c r="BQ21" s="13"/>
     </row>
-    <row r="22" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="22" spans="14:69">
       <c r="N22" s="11"/>
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
@@ -11140,7 +11161,7 @@
       <c r="BP22" s="12"/>
       <c r="BQ22" s="13"/>
     </row>
-    <row r="23" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="23" spans="14:69">
       <c r="N23" s="11"/>
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
@@ -11200,7 +11221,7 @@
       <c r="BP23" s="12"/>
       <c r="BQ23" s="13"/>
     </row>
-    <row r="24" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="24" spans="14:69">
       <c r="N24" s="11"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
@@ -11260,7 +11281,7 @@
       <c r="BP24" s="12"/>
       <c r="BQ24" s="13"/>
     </row>
-    <row r="25" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="25" spans="14:69">
       <c r="N25" s="11"/>
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
@@ -11322,7 +11343,7 @@
       <c r="BP25" s="12"/>
       <c r="BQ25" s="13"/>
     </row>
-    <row r="26" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="26" spans="14:69">
       <c r="N26" s="11"/>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
@@ -11384,7 +11405,7 @@
       <c r="BP26" s="12"/>
       <c r="BQ26" s="13"/>
     </row>
-    <row r="27" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="27" spans="14:69">
       <c r="N27" s="11"/>
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
@@ -11444,7 +11465,7 @@
       <c r="BP27" s="12"/>
       <c r="BQ27" s="13"/>
     </row>
-    <row r="28" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="28" spans="14:69">
       <c r="N28" s="11"/>
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
@@ -11504,7 +11525,7 @@
       <c r="BP28" s="12"/>
       <c r="BQ28" s="13"/>
     </row>
-    <row r="29" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="29" spans="14:69">
       <c r="N29" s="11"/>
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
@@ -11562,7 +11583,7 @@
       <c r="BP29" s="12"/>
       <c r="BQ29" s="13"/>
     </row>
-    <row r="30" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="30" spans="14:69">
       <c r="N30" s="11"/>
       <c r="O30" s="12"/>
       <c r="P30" s="12"/>
@@ -11620,7 +11641,7 @@
       <c r="BP30" s="12"/>
       <c r="BQ30" s="13"/>
     </row>
-    <row r="31" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="31" spans="14:69">
       <c r="N31" s="11"/>
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
@@ -11678,7 +11699,7 @@
       <c r="BP31" s="12"/>
       <c r="BQ31" s="13"/>
     </row>
-    <row r="32" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="32" spans="14:69">
       <c r="N32" s="11"/>
       <c r="O32" s="12"/>
       <c r="P32" s="12"/>
@@ -11736,7 +11757,7 @@
       <c r="BP32" s="12"/>
       <c r="BQ32" s="13"/>
     </row>
-    <row r="33" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="33" spans="14:69">
       <c r="N33" s="11"/>
       <c r="O33" s="12"/>
       <c r="P33" s="12"/>
@@ -11794,7 +11815,7 @@
       <c r="BP33" s="12"/>
       <c r="BQ33" s="13"/>
     </row>
-    <row r="34" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="34" spans="14:69">
       <c r="N34" s="11"/>
       <c r="O34" s="12"/>
       <c r="P34" s="12"/>
@@ -11856,7 +11877,7 @@
       <c r="BP34" s="12"/>
       <c r="BQ34" s="13"/>
     </row>
-    <row r="35" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="35" spans="14:69">
       <c r="N35" s="11"/>
       <c r="O35" s="12"/>
       <c r="P35" s="12"/>
@@ -11916,7 +11937,7 @@
       <c r="BP35" s="12"/>
       <c r="BQ35" s="13"/>
     </row>
-    <row r="36" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="36" spans="14:69">
       <c r="N36" s="11"/>
       <c r="O36" s="12"/>
       <c r="P36" s="12"/>
@@ -11975,7 +11996,7 @@
       <c r="BP36" s="12"/>
       <c r="BQ36" s="13"/>
     </row>
-    <row r="37" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="37" spans="14:69">
       <c r="N37" s="11"/>
       <c r="O37" s="12"/>
       <c r="P37" s="12"/>
@@ -12035,7 +12056,7 @@
       <c r="BP37" s="12"/>
       <c r="BQ37" s="13"/>
     </row>
-    <row r="38" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="38" spans="14:69">
       <c r="N38" s="11"/>
       <c r="O38" s="12"/>
       <c r="P38" s="12"/>
@@ -12095,7 +12116,7 @@
       <c r="BP38" s="12"/>
       <c r="BQ38" s="13"/>
     </row>
-    <row r="39" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="39" spans="14:69">
       <c r="N39" s="11"/>
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
@@ -12153,7 +12174,7 @@
       <c r="BP39" s="12"/>
       <c r="BQ39" s="13"/>
     </row>
-    <row r="40" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="40" spans="14:69">
       <c r="N40" s="11"/>
       <c r="O40" s="12"/>
       <c r="P40" s="12"/>
@@ -12211,7 +12232,7 @@
       <c r="BP40" s="12"/>
       <c r="BQ40" s="13"/>
     </row>
-    <row r="41" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="41" spans="14:69">
       <c r="N41" s="11"/>
       <c r="O41" s="12"/>
       <c r="P41" s="12"/>
@@ -12269,7 +12290,7 @@
       <c r="BP41" s="12"/>
       <c r="BQ41" s="13"/>
     </row>
-    <row r="42" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="42" spans="14:69">
       <c r="N42" s="11"/>
       <c r="O42" s="12"/>
       <c r="P42" s="12"/>
@@ -12327,7 +12348,7 @@
       <c r="BP42" s="12"/>
       <c r="BQ42" s="13"/>
     </row>
-    <row r="43" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="43" spans="14:69">
       <c r="N43" s="11"/>
       <c r="O43" s="12"/>
       <c r="P43" s="12"/>
@@ -12385,7 +12406,7 @@
       <c r="BP43" s="12"/>
       <c r="BQ43" s="13"/>
     </row>
-    <row r="44" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="44" spans="14:69">
       <c r="N44" s="11"/>
       <c r="O44" s="12"/>
       <c r="P44" s="12"/>
@@ -12443,7 +12464,7 @@
       <c r="BP44" s="12"/>
       <c r="BQ44" s="13"/>
     </row>
-    <row r="45" spans="14:69" x14ac:dyDescent="0.15">
+    <row r="45" spans="14:69">
       <c r="N45" s="11"/>
       <c r="O45" s="12"/>
       <c r="P45" s="12"/>
@@ -12503,7 +12524,7 @@
       <c r="BP45" s="12"/>
       <c r="BQ45" s="13"/>
     </row>
-    <row r="46" spans="14:69" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="14:69" ht="15.75" thickBot="1">
       <c r="N46" s="14"/>
       <c r="O46" s="15"/>
       <c r="P46" s="15"/>
@@ -12571,23 +12592,23 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:E28"/>
+  <dimension ref="C1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="4" width="9.125" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="3:6">
       <c r="C1" s="93" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="3:6">
       <c r="C2" s="6" t="s">
         <v>283</v>
       </c>
@@ -12597,8 +12618,11 @@
       <c r="E2" s="6" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F2" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="3" spans="3:6">
       <c r="C3" s="94" t="s">
         <v>252</v>
       </c>
@@ -12608,8 +12632,11 @@
       <c r="E3" s="56" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F3" s="114" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
       <c r="C4" s="56" t="s">
         <v>251</v>
       </c>
@@ -12619,8 +12646,11 @@
       <c r="E4" s="56" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F4" s="94" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
       <c r="C5" s="56" t="s">
         <v>253</v>
       </c>
@@ -12630,19 +12660,21 @@
       <c r="E5" s="56" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F5" s="56"/>
+    </row>
+    <row r="6" spans="3:6">
       <c r="C6" s="95" t="s">
         <v>255</v>
       </c>
       <c r="D6" s="56" t="s">
         <v>279</v>
       </c>
-      <c r="E6" s="94" t="s">
+      <c r="E6" s="116" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F6" s="56"/>
+    </row>
+    <row r="7" spans="3:6">
       <c r="C7" s="56" t="s">
         <v>258</v>
       </c>
@@ -12652,35 +12684,43 @@
       <c r="E7" s="56" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F7" s="56"/>
+    </row>
+    <row r="8" spans="3:6">
       <c r="C8" s="94" t="s">
         <v>259</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="94" t="s">
+      <c r="D8" s="56" t="s">
+        <v>486</v>
+      </c>
+      <c r="E8" s="116" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F8" s="56"/>
+    </row>
+    <row r="9" spans="3:6">
       <c r="C9" s="94" t="s">
         <v>260</v>
       </c>
-      <c r="D9" s="56"/>
+      <c r="D9" s="56" t="s">
+        <v>272</v>
+      </c>
       <c r="E9" s="94" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C10" s="94" t="s">
+      <c r="F9" s="56"/>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="C10" s="116" t="s">
         <v>261</v>
       </c>
       <c r="D10" s="56"/>
       <c r="E10" s="95" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F10" s="56"/>
+    </row>
+    <row r="11" spans="3:6">
       <c r="C11" s="56" t="s">
         <v>262</v>
       </c>
@@ -12688,8 +12728,9 @@
       <c r="E11" s="94" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F11" s="56"/>
+    </row>
+    <row r="12" spans="3:6">
       <c r="C12" s="56" t="s">
         <v>264</v>
       </c>
@@ -12697,8 +12738,9 @@
       <c r="E12" s="56" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F12" s="56"/>
+    </row>
+    <row r="13" spans="3:6">
       <c r="C13" s="56" t="s">
         <v>265</v>
       </c>
@@ -12706,8 +12748,9 @@
       <c r="E13" s="56" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F13" s="56"/>
+    </row>
+    <row r="14" spans="3:6">
       <c r="C14" s="56" t="s">
         <v>266</v>
       </c>
@@ -12715,89 +12758,134 @@
       <c r="E14" s="56" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F14" s="56"/>
+    </row>
+    <row r="15" spans="3:6">
       <c r="C15" s="94" t="s">
         <v>267</v>
       </c>
       <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="E15" s="56" t="s">
+        <v>487</v>
+      </c>
+      <c r="F15" s="56"/>
+    </row>
+    <row r="16" spans="3:6">
       <c r="C16" s="56" t="s">
         <v>268</v>
       </c>
       <c r="D16" s="56"/>
       <c r="E16" s="56"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C17" s="94" t="s">
+      <c r="F16" s="56"/>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="C17" s="116" t="s">
         <v>269</v>
       </c>
       <c r="D17" s="56"/>
       <c r="E17" s="56"/>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F17" s="56"/>
+    </row>
+    <row r="18" spans="3:6">
       <c r="C18" s="56" t="s">
         <v>273</v>
       </c>
       <c r="D18" s="56"/>
       <c r="E18" s="56"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F18" s="56"/>
+    </row>
+    <row r="19" spans="3:6">
       <c r="C19" s="56" t="s">
         <v>256</v>
       </c>
       <c r="D19" s="56"/>
       <c r="E19" s="56"/>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="F19" s="56"/>
+    </row>
+    <row r="20" spans="3:6">
       <c r="C20" s="115" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+    </row>
+    <row r="21" spans="3:6">
       <c r="C21" s="114" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+    </row>
+    <row r="22" spans="3:6">
       <c r="C22" s="114" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+    </row>
+    <row r="23" spans="3:6">
       <c r="C23" s="115" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+    </row>
+    <row r="24" spans="3:6">
       <c r="C24" s="114" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+    </row>
+    <row r="25" spans="3:6">
       <c r="C25" s="114" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+    </row>
+    <row r="26" spans="3:6">
       <c r="C26" s="115" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+    </row>
+    <row r="27" spans="3:6">
       <c r="C27" s="114" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C28" s="114" t="s">
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28" s="117" t="s">
         <v>482</v>
+      </c>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+    </row>
+    <row r="29" spans="3:6">
+      <c r="C29" s="114" t="s">
+        <v>489</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M10">
+      <formula1>"1,2,3"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -12811,132 +12899,132 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="79.25" customWidth="1"/>
+    <col min="2" max="2" width="79.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:2" ht="18" customHeight="1">
       <c r="B2" s="96" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:2" ht="18" customHeight="1">
       <c r="B3" s="96" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:2" ht="18" customHeight="1">
       <c r="B4" s="96" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:2" ht="18" customHeight="1">
       <c r="B5" s="96" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:2" ht="18" customHeight="1">
       <c r="B6" s="96" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:2" ht="18" customHeight="1">
       <c r="B7" s="96" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:2" ht="18" customHeight="1">
       <c r="B8" s="96" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:2" ht="18" customHeight="1">
       <c r="B9" s="96" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:2" ht="18" customHeight="1">
       <c r="B10" s="96" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:2" ht="18" customHeight="1">
       <c r="B11" s="96" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:2" ht="18" customHeight="1">
       <c r="B12" s="96" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:2" ht="18" customHeight="1">
       <c r="B13" s="96" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:2" ht="18" customHeight="1">
       <c r="B14" s="96" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:2" ht="18" customHeight="1">
       <c r="B15" s="96" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="16" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:2" ht="18" customHeight="1">
       <c r="B16" s="105" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" ht="18" customHeight="1">
       <c r="B17" s="105" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" ht="18" customHeight="1">
       <c r="B18" s="96" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" ht="18" customHeight="1">
       <c r="B19" s="105" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" ht="18" customHeight="1">
       <c r="B20" s="96" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" ht="18" customHeight="1">
       <c r="B21" s="96" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" ht="18" customHeight="1">
       <c r="B22" s="105" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2" ht="18" customHeight="1">
       <c r="B23" s="96" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:2" ht="18" customHeight="1">
       <c r="B24" s="96" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:2" ht="18" customHeight="1">
       <c r="B25" s="96" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:2" ht="18" customHeight="1">
       <c r="B26" s="96" t="s">
         <v>321</v>
       </c>
@@ -12956,49 +13044,49 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:2" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:2" ht="22.5">
       <c r="B2" s="98" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:2">
       <c r="B3" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:2">
       <c r="B10" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:2">
       <c r="B13" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:2">
       <c r="B15" t="s">
         <v>339</v>
       </c>
@@ -13018,9 +13106,9 @@
       <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:9">
       <c r="B2" s="104" t="s">
         <v>332</v>
       </c>
@@ -13038,7 +13126,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>390</v>
       </c>
@@ -13058,12 +13146,12 @@
       <selection activeCell="BR25" sqref="BR25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="3" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="3" style="7"/>
   </cols>
   <sheetData>
-    <row r="4" spans="10:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="10:13">
       <c r="J4" s="7" t="s">
         <v>336</v>
       </c>
@@ -13071,37 +13159,37 @@
         <v>338</v>
       </c>
     </row>
-    <row r="5" spans="10:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="10:13">
       <c r="M5" s="7" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="7" spans="10:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="10:13">
       <c r="M7" s="7" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="11" spans="10:13" x14ac:dyDescent="0.15">
+    <row r="11" spans="10:13">
       <c r="J11" s="7" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="12" spans="10:13" x14ac:dyDescent="0.15">
+    <row r="12" spans="10:13">
       <c r="J12" s="7" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="13" spans="10:13" x14ac:dyDescent="0.15">
+    <row r="13" spans="10:13">
       <c r="J13" s="7" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="14" spans="10:13" x14ac:dyDescent="0.15">
+    <row r="14" spans="10:13">
       <c r="J14" s="7" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="18" spans="10:21" x14ac:dyDescent="0.15">
+    <row r="18" spans="10:21">
       <c r="J18" s="7" t="s">
         <v>342</v>
       </c>
@@ -13122,25 +13210,25 @@
         <v>335</v>
       </c>
     </row>
-    <row r="19" spans="10:21" x14ac:dyDescent="0.15">
+    <row r="19" spans="10:21">
       <c r="J19" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="22" spans="10:21" x14ac:dyDescent="0.15">
+    <row r="22" spans="10:21">
       <c r="K22" s="99"/>
     </row>
-    <row r="23" spans="10:21" x14ac:dyDescent="0.15">
+    <row r="23" spans="10:21">
       <c r="J23" s="7" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="24" spans="10:21" x14ac:dyDescent="0.15">
+    <row r="24" spans="10:21">
       <c r="J24" s="7" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="25" spans="10:21" x14ac:dyDescent="0.15">
+    <row r="25" spans="10:21">
       <c r="J25" s="7" t="s">
         <v>346</v>
       </c>
@@ -13160,44 +13248,44 @@
       <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:2">
       <c r="B2" s="97" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:2">
       <c r="B3" s="97" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:2">
       <c r="B4" s="97" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:2" ht="34.5">
       <c r="B7" s="101" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:2">
       <c r="B8" s="103" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:2">
       <c r="B9" s="100" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:2" ht="30">
       <c r="B10" s="102" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:2">
       <c r="B11" s="100" t="s">
         <v>355</v>
       </c>
@@ -13222,182 +13310,182 @@
       <selection activeCell="AG24" sqref="AG24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.375" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="3.375" style="7"/>
+    <col min="1" max="16384" width="3.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="4:4">
       <c r="D3" s="64" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="4:4">
       <c r="D4" s="7" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="5" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="4:4">
       <c r="D5" s="7" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="7" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="4:4">
       <c r="D7" s="64" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="4:4">
       <c r="D8" s="7" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="9" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="4:4">
       <c r="D9" s="7" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="4:4">
       <c r="D10" s="7" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="11" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="4:4">
       <c r="D11" s="7" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="13" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="4:4">
       <c r="D13" s="64" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="14" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="4:4">
       <c r="D14" s="7" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="16" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="4:4">
       <c r="D16" s="64" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="4:5">
       <c r="D17" s="7" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="4:5">
       <c r="D19" s="64" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="4:5">
       <c r="D20" s="7" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="4:5">
       <c r="D22" s="64" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="4:5">
       <c r="D23" s="7" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="4:5">
       <c r="D25" s="64" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="4:5">
       <c r="D26" s="7" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="4:5">
       <c r="D28" s="64" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="4:5">
       <c r="D29" s="7" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="4:5">
       <c r="E30" s="7" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="4:5">
       <c r="E31" s="7" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="4:5">
       <c r="E32" s="7" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="4:5">
       <c r="D34" s="64" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="4:5">
       <c r="D35" s="7" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="4:5">
       <c r="E36" s="7" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="4:5">
       <c r="D38" s="64" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="4:5">
       <c r="D39" s="7" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="4:5">
       <c r="D40" s="7" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="4:5">
       <c r="D42" s="64" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="4:5">
       <c r="D43" s="7" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="44" spans="4:5">
       <c r="D44" s="7" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="45" spans="4:5">
       <c r="D45" s="7" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="47" spans="4:5">
       <c r="D47" s="64" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="48" spans="4:5">
       <c r="D48" s="7" t="s">
         <v>388</v>
       </c>
@@ -13416,12 +13504,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="2.875" style="7"/>
+    <col min="1" max="16384" width="2.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" ht="36.75" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:27" ht="35.25">
       <c r="E2" s="12" t="s">
         <v>408</v>
       </c>
@@ -13442,7 +13530,7 @@
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
     </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:27">
       <c r="E3" s="7" t="s">
         <v>410</v>
       </c>
@@ -13450,7 +13538,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="6" spans="2:27" ht="20.25" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:27" ht="21">
       <c r="B6" s="110"/>
       <c r="C6" s="110"/>
       <c r="D6" s="110"/>
@@ -13471,7 +13559,7 @@
       <c r="Q6" s="111"/>
       <c r="R6" s="111"/>
     </row>
-    <row r="7" spans="2:27" ht="20.25" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:27" ht="21">
       <c r="B7" s="110"/>
       <c r="C7" s="110"/>
       <c r="D7" s="110"/>
@@ -13489,7 +13577,7 @@
       <c r="Q7" s="111"/>
       <c r="R7" s="111"/>
     </row>
-    <row r="8" spans="2:27" ht="20.25" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:27" ht="21">
       <c r="B8" s="112"/>
       <c r="C8" s="112"/>
       <c r="D8" s="110"/>
@@ -13507,24 +13595,24 @@
       <c r="Q8" s="111"/>
       <c r="R8" s="111"/>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:27">
       <c r="B9" s="112"/>
       <c r="C9" s="112" t="s">
         <v>416</v>
       </c>
       <c r="D9" s="110"/>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:27">
       <c r="B10" s="112"/>
       <c r="C10" s="112"/>
       <c r="D10" s="110"/>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:27">
       <c r="B11" s="112"/>
       <c r="C11" s="112"/>
       <c r="D11" s="110"/>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:27">
       <c r="B12" s="112"/>
       <c r="C12" s="112" t="s">
         <v>417</v>
@@ -13538,7 +13626,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:27">
       <c r="B13" s="112"/>
       <c r="C13" s="112"/>
       <c r="D13" s="110"/>
@@ -13546,7 +13634,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:27">
       <c r="B14" s="112"/>
       <c r="C14" s="112"/>
       <c r="D14" s="110"/>
@@ -13554,7 +13642,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:27">
       <c r="B15" s="112"/>
       <c r="C15" s="112"/>
       <c r="D15" s="110"/>
@@ -13562,7 +13650,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:27">
       <c r="B16" s="112"/>
       <c r="C16" s="112"/>
       <c r="D16" s="110"/>
@@ -13570,7 +13658,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7">
       <c r="B17" s="112"/>
       <c r="C17" s="112"/>
       <c r="D17" s="110"/>
@@ -13578,7 +13666,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:7">
       <c r="B18" s="110"/>
       <c r="C18" s="110"/>
       <c r="D18" s="110"/>
@@ -13586,7 +13674,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:7">
       <c r="B19" s="110"/>
       <c r="C19" s="110"/>
       <c r="D19" s="110"/>
@@ -13594,7 +13682,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:7">
       <c r="B20" s="110"/>
       <c r="C20" s="110"/>
       <c r="D20" s="110"/>
@@ -13602,7 +13690,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:7">
       <c r="B21" s="110"/>
       <c r="C21" s="110"/>
       <c r="D21" s="110"/>
@@ -13610,7 +13698,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:7">
       <c r="B22" s="110"/>
       <c r="C22" s="110"/>
       <c r="D22" s="110"/>
@@ -13618,7 +13706,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:7">
       <c r="B23" s="110"/>
       <c r="C23" s="110"/>
       <c r="D23" s="110"/>
@@ -13626,7 +13714,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:7">
       <c r="B24" s="110"/>
       <c r="C24" s="110"/>
       <c r="D24" s="110"/>
@@ -13634,7 +13722,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:7">
       <c r="B25" s="110"/>
       <c r="C25" s="110"/>
       <c r="D25" s="110"/>
@@ -13642,7 +13730,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:7">
       <c r="B26" s="110"/>
       <c r="C26" s="110"/>
       <c r="D26" s="110"/>
@@ -13650,7 +13738,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:7">
       <c r="B27" s="110"/>
       <c r="C27" s="110"/>
       <c r="D27" s="110"/>
@@ -13658,12 +13746,12 @@
         <v>434</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:7">
       <c r="B28" s="110"/>
       <c r="C28" s="110"/>
       <c r="D28" s="110"/>
     </row>
-    <row r="35" spans="2:10" ht="20.25" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:10" ht="21">
       <c r="B35" s="112"/>
       <c r="C35" s="112"/>
       <c r="D35" s="112"/>
@@ -13673,7 +13761,7 @@
       <c r="I35" s="111"/>
       <c r="J35" s="111"/>
     </row>
-    <row r="36" spans="2:10" ht="20.25" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:10" ht="21">
       <c r="B36" s="112"/>
       <c r="C36" s="112"/>
       <c r="D36" s="112"/>
@@ -13682,12 +13770,12 @@
       </c>
       <c r="J36" s="111"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:10">
       <c r="B37" s="112"/>
       <c r="C37" s="112"/>
       <c r="D37" s="112"/>
     </row>
-    <row r="38" spans="2:10" ht="20.25" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:10" ht="21">
       <c r="B38" s="112"/>
       <c r="C38" s="112"/>
       <c r="D38" s="112"/>
@@ -13696,7 +13784,7 @@
       </c>
       <c r="I38" s="111"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:10">
       <c r="B39" s="112"/>
       <c r="C39" s="112" t="s">
         <v>437</v>
@@ -13706,7 +13794,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:10">
       <c r="B40" s="112"/>
       <c r="C40" s="112"/>
       <c r="D40" s="112"/>
@@ -13714,7 +13802,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:10">
       <c r="B41" s="112"/>
       <c r="C41" s="112"/>
       <c r="D41" s="112"/>
@@ -13722,17 +13810,17 @@
         <v>440</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:10">
       <c r="B42" s="112"/>
       <c r="C42" s="112"/>
       <c r="D42" s="112"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:10">
       <c r="B43" s="112"/>
       <c r="C43" s="112"/>
       <c r="D43" s="112"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:10">
       <c r="B44" s="112"/>
       <c r="C44" s="112"/>
       <c r="D44" s="112"/>
@@ -13740,12 +13828,12 @@
         <v>441</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:10">
       <c r="B45" s="112"/>
       <c r="C45" s="112"/>
       <c r="D45" s="112"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:10">
       <c r="B46" s="112"/>
       <c r="C46" s="112"/>
       <c r="D46" s="112"/>
@@ -13753,7 +13841,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:10">
       <c r="B47" s="112"/>
       <c r="C47" s="112"/>
       <c r="D47" s="112"/>
@@ -13761,7 +13849,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:10">
       <c r="B48" s="112"/>
       <c r="C48" s="112"/>
       <c r="D48" s="112"/>
@@ -13769,7 +13857,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:13">
       <c r="B49" s="112"/>
       <c r="C49" s="112"/>
       <c r="D49" s="112"/>
@@ -13777,12 +13865,12 @@
         <v>445</v>
       </c>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:13">
       <c r="B50" s="112"/>
       <c r="C50" s="112"/>
       <c r="D50" s="112"/>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:13">
       <c r="B51" s="112"/>
       <c r="C51" s="112"/>
       <c r="D51" s="112"/>
@@ -13790,12 +13878,12 @@
         <v>446</v>
       </c>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:13">
       <c r="B52" s="112"/>
       <c r="C52" s="112"/>
       <c r="D52" s="112"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:13">
       <c r="B53" s="112"/>
       <c r="C53" s="112"/>
       <c r="D53" s="112"/>
@@ -13803,7 +13891,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:13">
       <c r="B54" s="112"/>
       <c r="C54" s="112"/>
       <c r="D54" s="112"/>
@@ -13811,12 +13899,12 @@
         <v>448</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:13">
       <c r="B55" s="112"/>
       <c r="C55" s="112"/>
       <c r="D55" s="112"/>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:13">
       <c r="B56" s="112"/>
       <c r="C56" s="112"/>
       <c r="D56" s="112"/>
@@ -13824,13 +13912,13 @@
         <v>449</v>
       </c>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:13">
       <c r="B57" s="112"/>
       <c r="C57" s="112"/>
       <c r="D57" s="112"/>
       <c r="M57" s="64"/>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:13">
       <c r="B58" s="112"/>
       <c r="C58" s="112"/>
       <c r="D58" s="112"/>
@@ -13838,7 +13926,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:13">
       <c r="B59" s="112"/>
       <c r="C59" s="112"/>
       <c r="D59" s="112"/>
@@ -13846,83 +13934,83 @@
         <v>451</v>
       </c>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:13">
       <c r="B60" s="112"/>
       <c r="C60" s="112"/>
       <c r="D60" s="112"/>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:13">
       <c r="B61" s="112"/>
       <c r="C61" s="112"/>
       <c r="D61" s="112"/>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:13">
       <c r="B62" s="112"/>
       <c r="C62" s="112"/>
       <c r="D62" s="112"/>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:13">
       <c r="B63" s="112"/>
       <c r="C63" s="112"/>
       <c r="D63" s="112"/>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:13">
       <c r="B64" s="112"/>
       <c r="C64" s="112"/>
       <c r="D64" s="112"/>
     </row>
-    <row r="65" spans="2:28" x14ac:dyDescent="0.15">
+    <row r="65" spans="2:28">
       <c r="B65" s="112"/>
       <c r="C65" s="112"/>
       <c r="D65" s="112"/>
     </row>
-    <row r="66" spans="2:28" x14ac:dyDescent="0.15">
+    <row r="66" spans="2:28">
       <c r="B66" s="112"/>
       <c r="C66" s="112"/>
       <c r="D66" s="112"/>
     </row>
-    <row r="67" spans="2:28" x14ac:dyDescent="0.15">
+    <row r="67" spans="2:28">
       <c r="B67" s="112"/>
       <c r="C67" s="112"/>
       <c r="D67" s="112"/>
     </row>
-    <row r="68" spans="2:28" x14ac:dyDescent="0.15">
+    <row r="68" spans="2:28">
       <c r="B68" s="112"/>
       <c r="C68" s="112"/>
       <c r="D68" s="112"/>
       <c r="AB68"/>
     </row>
-    <row r="69" spans="2:28" x14ac:dyDescent="0.15">
+    <row r="69" spans="2:28">
       <c r="B69" s="112"/>
       <c r="C69" s="112"/>
       <c r="D69" s="112"/>
     </row>
-    <row r="70" spans="2:28" x14ac:dyDescent="0.15">
+    <row r="70" spans="2:28">
       <c r="B70" s="112"/>
       <c r="C70" s="112"/>
       <c r="D70" s="112"/>
     </row>
-    <row r="71" spans="2:28" x14ac:dyDescent="0.15">
+    <row r="71" spans="2:28">
       <c r="B71" s="112"/>
       <c r="C71" s="112"/>
       <c r="D71" s="112"/>
     </row>
-    <row r="72" spans="2:28" x14ac:dyDescent="0.15">
+    <row r="72" spans="2:28">
       <c r="B72" s="112"/>
       <c r="C72" s="112"/>
       <c r="D72" s="112"/>
     </row>
-    <row r="73" spans="2:28" x14ac:dyDescent="0.15">
+    <row r="73" spans="2:28">
       <c r="B73" s="112"/>
       <c r="C73" s="112"/>
       <c r="D73" s="112"/>
     </row>
-    <row r="74" spans="2:28" x14ac:dyDescent="0.15">
+    <row r="74" spans="2:28">
       <c r="B74" s="112"/>
       <c r="C74" s="112"/>
       <c r="D74" s="112"/>
     </row>
-    <row r="75" spans="2:28" x14ac:dyDescent="0.15">
+    <row r="75" spans="2:28">
       <c r="B75" s="112"/>
       <c r="C75" s="112"/>
       <c r="D75" s="112"/>
@@ -13942,9 +14030,9 @@
       <selection activeCell="Y43" sqref="Y43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:4">
       <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
@@ -13955,7 +14043,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4">
       <c r="B2" s="6" t="s">
         <v>27</v>
       </c>
@@ -13978,27 +14066,27 @@
       <selection activeCell="AL31" sqref="AL31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="2.75" style="7"/>
+    <col min="1" max="16384" width="2.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="3" spans="4:30">
       <c r="D3" s="7" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="5" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="5" spans="4:30">
       <c r="E5" s="7" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="7" spans="4:30">
       <c r="E7" s="7" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="15" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="15" spans="4:30">
       <c r="E15" s="113" t="s">
         <v>455</v>
       </c>
@@ -14006,22 +14094,22 @@
         <v>456</v>
       </c>
     </row>
-    <row r="16" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="16" spans="4:30">
       <c r="AD16" s="7" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="17" spans="7:30" x14ac:dyDescent="0.15">
+    <row r="17" spans="7:30">
       <c r="AD17" s="7" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="18" spans="7:30" x14ac:dyDescent="0.15">
+    <row r="18" spans="7:30">
       <c r="AD18" s="7" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="19" spans="7:30" x14ac:dyDescent="0.15">
+    <row r="19" spans="7:30">
       <c r="G19" s="7" t="s">
         <v>458</v>
       </c>
@@ -14029,37 +14117,37 @@
         <v>459</v>
       </c>
     </row>
-    <row r="20" spans="7:30" x14ac:dyDescent="0.15">
+    <row r="20" spans="7:30">
       <c r="J20" s="7" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="22" spans="7:30" x14ac:dyDescent="0.15">
+    <row r="22" spans="7:30">
       <c r="J22" s="7" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="26" spans="7:30" x14ac:dyDescent="0.15">
+    <row r="26" spans="7:30">
       <c r="G26" s="7" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="27" spans="7:30" x14ac:dyDescent="0.15">
+    <row r="27" spans="7:30">
       <c r="G27" s="7" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="28" spans="7:30" x14ac:dyDescent="0.15">
+    <row r="28" spans="7:30">
       <c r="G28" s="7" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="29" spans="7:30" x14ac:dyDescent="0.15">
+    <row r="29" spans="7:30">
       <c r="G29" s="7" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="33" spans="7:18" x14ac:dyDescent="0.15">
+    <row r="33" spans="7:18">
       <c r="G33" s="7" t="s">
         <v>466</v>
       </c>
@@ -14080,25 +14168,25 @@
         <v>470</v>
       </c>
     </row>
-    <row r="34" spans="7:18" x14ac:dyDescent="0.15">
+    <row r="34" spans="7:18">
       <c r="G34" s="7" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="37" spans="7:18" x14ac:dyDescent="0.15">
+    <row r="37" spans="7:18">
       <c r="H37" s="99"/>
     </row>
-    <row r="38" spans="7:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="7:18">
       <c r="G38" s="7" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="39" spans="7:18" x14ac:dyDescent="0.15">
+    <row r="39" spans="7:18">
       <c r="G39" s="7" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="40" spans="7:18" x14ac:dyDescent="0.15">
+    <row r="40" spans="7:18">
       <c r="G40" s="7" t="s">
         <v>474</v>
       </c>
@@ -14118,9 +14206,9 @@
       <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:4">
       <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
@@ -14131,7 +14219,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4">
       <c r="B2" s="6" t="s">
         <v>31</v>
       </c>
@@ -14154,9 +14242,9 @@
       <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:4">
       <c r="B1" t="s">
         <v>33</v>
       </c>
@@ -14167,7 +14255,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
         <v>36</v>
       </c>
@@ -14187,7 +14275,7 @@
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14203,17 +14291,17 @@
       <selection activeCell="AB32" sqref="AB32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="79" width="2.625" style="7"/>
-    <col min="80" max="80" width="3.625" style="7" customWidth="1"/>
-    <col min="81" max="83" width="2.625" style="7"/>
-    <col min="84" max="84" width="8.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="85" max="16384" width="2.625" style="7"/>
+    <col min="1" max="79" width="2.5703125" style="7"/>
+    <col min="80" max="80" width="3.5703125" style="7" customWidth="1"/>
+    <col min="81" max="83" width="2.5703125" style="7"/>
+    <col min="84" max="84" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="85" max="16384" width="2.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:90" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="2" spans="4:90" ht="15.75" thickBot="1"/>
+    <row r="3" spans="4:90">
       <c r="D3" s="8"/>
       <c r="E3" s="9" t="s">
         <v>322</v>
@@ -14292,7 +14380,7 @@
       <c r="CA3" s="22"/>
       <c r="CB3" s="23"/>
     </row>
-    <row r="4" spans="4:90" ht="20.25" x14ac:dyDescent="0.15">
+    <row r="4" spans="4:90" ht="21">
       <c r="D4" s="11"/>
       <c r="E4" s="97" t="s">
         <v>323</v>
@@ -14381,7 +14469,7 @@
       <c r="CA4" s="27"/>
       <c r="CB4" s="26"/>
     </row>
-    <row r="5" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="5" spans="4:90">
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
@@ -14458,7 +14546,7 @@
       <c r="CA5" s="25"/>
       <c r="CB5" s="26"/>
     </row>
-    <row r="6" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="6" spans="4:90">
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -14535,7 +14623,7 @@
       <c r="CA6" s="12"/>
       <c r="CB6" s="13"/>
     </row>
-    <row r="7" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="7" spans="4:90">
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -14617,7 +14705,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="8" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="8" spans="4:90">
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
@@ -14697,7 +14785,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="9" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="9" spans="4:90">
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
@@ -14777,7 +14865,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="10" spans="4:90">
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -14857,7 +14945,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="11" spans="4:90">
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -14948,7 +15036,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="12" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="12" spans="4:90">
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -15028,7 +15116,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="13" spans="4:90">
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
@@ -15111,7 +15199,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="14" spans="4:90">
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -15190,7 +15278,7 @@
       <c r="CA14" s="31"/>
       <c r="CB14" s="13"/>
     </row>
-    <row r="15" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="15" spans="4:90">
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12" t="s">
@@ -15272,7 +15360,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="16" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="16" spans="4:90">
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12" t="s">
@@ -15354,7 +15442,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="17" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="17" spans="4:90">
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -15434,7 +15522,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="18" spans="4:90">
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -15511,7 +15599,7 @@
       <c r="CA18" s="31"/>
       <c r="CB18" s="13"/>
     </row>
-    <row r="19" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="19" spans="4:90">
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
@@ -15588,7 +15676,7 @@
       <c r="CA19" s="31"/>
       <c r="CB19" s="13"/>
     </row>
-    <row r="20" spans="4:90" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:90" ht="15.75" thickBot="1">
       <c r="D20" s="14"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -15665,7 +15753,7 @@
       <c r="CA20" s="31"/>
       <c r="CB20" s="13"/>
     </row>
-    <row r="21" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="21" spans="4:90">
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -15737,7 +15825,7 @@
       <c r="CA21" s="31"/>
       <c r="CB21" s="13"/>
     </row>
-    <row r="22" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="22" spans="4:90">
       <c r="U22" s="7" t="s">
         <v>186</v>
       </c>
@@ -15788,7 +15876,7 @@
       <c r="CA22" s="31"/>
       <c r="CB22" s="13"/>
     </row>
-    <row r="23" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="23" spans="4:90">
       <c r="I23" s="7" t="s">
         <v>201</v>
       </c>
@@ -15844,7 +15932,7 @@
       <c r="CA23" s="41"/>
       <c r="CB23" s="13"/>
     </row>
-    <row r="24" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="24" spans="4:90">
       <c r="I24" s="7" t="s">
         <v>202</v>
       </c>
@@ -15898,7 +15986,7 @@
       <c r="CA24" s="31"/>
       <c r="CB24" s="13"/>
     </row>
-    <row r="25" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="25" spans="4:90">
       <c r="N25" s="7" t="s">
         <v>204</v>
       </c>
@@ -15952,7 +16040,7 @@
       <c r="CA25" s="31"/>
       <c r="CB25" s="13"/>
     </row>
-    <row r="26" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="26" spans="4:90">
       <c r="N26" s="7" t="s">
         <v>205</v>
       </c>
@@ -16003,7 +16091,7 @@
       <c r="CA26" s="34"/>
       <c r="CB26" s="13"/>
     </row>
-    <row r="27" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="27" spans="4:90">
       <c r="U27" s="7" t="s">
         <v>200</v>
       </c>
@@ -16054,7 +16142,7 @@
       <c r="CA27" s="12"/>
       <c r="CB27" s="13"/>
     </row>
-    <row r="28" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="28" spans="4:90">
       <c r="AI28" s="11"/>
       <c r="AJ28" s="30"/>
       <c r="AK28" s="47"/>
@@ -16102,7 +16190,7 @@
       <c r="CA28" s="12"/>
       <c r="CB28" s="13"/>
     </row>
-    <row r="29" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="29" spans="4:90">
       <c r="AI29" s="11"/>
       <c r="AJ29" s="30"/>
       <c r="AK29" s="12"/>
@@ -16150,7 +16238,7 @@
       <c r="CA29" s="12"/>
       <c r="CB29" s="13"/>
     </row>
-    <row r="30" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="30" spans="4:90">
       <c r="AI30" s="11"/>
       <c r="AJ30" s="30"/>
       <c r="AK30" s="42"/>
@@ -16198,7 +16286,7 @@
       <c r="CA30" s="12"/>
       <c r="CB30" s="13"/>
     </row>
-    <row r="31" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="31" spans="4:90">
       <c r="AI31" s="11"/>
       <c r="AJ31" s="30"/>
       <c r="AK31" s="45"/>
@@ -16246,7 +16334,7 @@
       <c r="CA31" s="12"/>
       <c r="CB31" s="13"/>
     </row>
-    <row r="32" spans="4:90" x14ac:dyDescent="0.15">
+    <row r="32" spans="4:90">
       <c r="AI32" s="11"/>
       <c r="AJ32" s="30"/>
       <c r="AK32" s="45"/>
@@ -16294,7 +16382,7 @@
       <c r="CA32" s="12"/>
       <c r="CB32" s="13"/>
     </row>
-    <row r="33" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="33" spans="35:80">
       <c r="AI33" s="11"/>
       <c r="AJ33" s="30"/>
       <c r="AK33" s="45"/>
@@ -16342,7 +16430,7 @@
       <c r="CA33" s="12"/>
       <c r="CB33" s="13"/>
     </row>
-    <row r="34" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="34" spans="35:80">
       <c r="AI34" s="11"/>
       <c r="AJ34" s="30"/>
       <c r="AK34" s="45"/>
@@ -16390,7 +16478,7 @@
       <c r="CA34" s="12"/>
       <c r="CB34" s="13"/>
     </row>
-    <row r="35" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="35" spans="35:80">
       <c r="AI35" s="11"/>
       <c r="AJ35" s="30"/>
       <c r="AK35" s="45"/>
@@ -16438,7 +16526,7 @@
       <c r="CA35" s="12"/>
       <c r="CB35" s="13"/>
     </row>
-    <row r="36" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="36" spans="35:80">
       <c r="AI36" s="11"/>
       <c r="AJ36" s="30"/>
       <c r="AK36" s="47"/>
@@ -16486,7 +16574,7 @@
       <c r="CA36" s="12"/>
       <c r="CB36" s="13"/>
     </row>
-    <row r="37" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="37" spans="35:80">
       <c r="AI37" s="11"/>
       <c r="AJ37" s="32"/>
       <c r="AK37" s="33"/>
@@ -16534,7 +16622,7 @@
       <c r="CA37" s="12"/>
       <c r="CB37" s="13"/>
     </row>
-    <row r="38" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="38" spans="35:80">
       <c r="AI38" s="11"/>
       <c r="AJ38" s="12"/>
       <c r="AK38" s="12"/>
@@ -16582,7 +16670,7 @@
       <c r="CA38" s="12"/>
       <c r="CB38" s="13"/>
     </row>
-    <row r="39" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="39" spans="35:80">
       <c r="AI39" s="11"/>
       <c r="AJ39" s="12"/>
       <c r="AK39" s="12"/>
@@ -16630,7 +16718,7 @@
       <c r="CA39" s="12"/>
       <c r="CB39" s="13"/>
     </row>
-    <row r="40" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="40" spans="35:80">
       <c r="AI40" s="11"/>
       <c r="AJ40" s="12"/>
       <c r="AK40" s="12"/>
@@ -16678,7 +16766,7 @@
       <c r="CA40" s="12"/>
       <c r="CB40" s="13"/>
     </row>
-    <row r="41" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="41" spans="35:80">
       <c r="AI41" s="11"/>
       <c r="AJ41" s="12"/>
       <c r="AK41" s="12"/>
@@ -16726,7 +16814,7 @@
       <c r="CA41" s="12"/>
       <c r="CB41" s="13"/>
     </row>
-    <row r="42" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="42" spans="35:80">
       <c r="AI42" s="11"/>
       <c r="AJ42" s="12"/>
       <c r="AK42" s="12"/>
@@ -16774,7 +16862,7 @@
       <c r="CA42" s="12"/>
       <c r="CB42" s="13"/>
     </row>
-    <row r="43" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="43" spans="35:80">
       <c r="AI43" s="11"/>
       <c r="AJ43" s="12"/>
       <c r="AK43" s="12"/>
@@ -16822,7 +16910,7 @@
       <c r="CA43" s="12"/>
       <c r="CB43" s="13"/>
     </row>
-    <row r="44" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="44" spans="35:80">
       <c r="AI44" s="11"/>
       <c r="AJ44" s="12"/>
       <c r="AK44" s="12"/>
@@ -16870,7 +16958,7 @@
       <c r="CA44" s="12"/>
       <c r="CB44" s="13"/>
     </row>
-    <row r="45" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="45" spans="35:80">
       <c r="AI45" s="18"/>
       <c r="AJ45" s="19"/>
       <c r="AK45" s="19"/>
@@ -16918,7 +17006,7 @@
       <c r="CA45" s="19"/>
       <c r="CB45" s="20"/>
     </row>
-    <row r="46" spans="35:80" x14ac:dyDescent="0.15">
+    <row r="46" spans="35:80">
       <c r="AI46" s="18"/>
       <c r="AJ46" s="19" t="s">
         <v>47</v>
@@ -16976,7 +17064,7 @@
       <c r="CA46" s="19"/>
       <c r="CB46" s="20"/>
     </row>
-    <row r="47" spans="35:80" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="35:80" ht="15.75" thickBot="1">
       <c r="AI47" s="50"/>
       <c r="AJ47" s="51"/>
       <c r="AK47" s="51"/>
@@ -17043,14 +17131,14 @@
       <selection activeCell="BG40" sqref="BG40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="36" width="3.25" style="7"/>
-    <col min="37" max="37" width="7.125" style="7" customWidth="1"/>
-    <col min="38" max="16384" width="3.25" style="7"/>
+    <col min="1" max="36" width="3.28515625" style="7"/>
+    <col min="37" max="37" width="7.140625" style="7" customWidth="1"/>
+    <col min="38" max="16384" width="3.28515625" style="7"/>
   </cols>
   <sheetData>
-    <row r="4" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="4" spans="8:66">
       <c r="H4" s="64" t="s">
         <v>221</v>
       </c>
@@ -17087,7 +17175,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="5" spans="8:66">
       <c r="H5" s="7" t="s">
         <v>222</v>
       </c>
@@ -17125,7 +17213,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="6" spans="8:66">
       <c r="H6" s="7" t="s">
         <v>223</v>
       </c>
@@ -17148,7 +17236,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="7" spans="8:66">
       <c r="H7" s="7" t="s">
         <v>224</v>
       </c>
@@ -17165,7 +17253,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="8" spans="8:66">
       <c r="I8" s="7" t="s">
         <v>225</v>
       </c>
@@ -17182,7 +17270,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="9" spans="8:66">
       <c r="I9" s="7" t="s">
         <v>226</v>
       </c>
@@ -17196,7 +17284,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="10" spans="8:66">
       <c r="I10" s="7" t="s">
         <v>227</v>
       </c>
@@ -17207,7 +17295,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="11" spans="8:66">
       <c r="I11" s="7" t="s">
         <v>228</v>
       </c>
@@ -17221,7 +17309,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="12" spans="8:66">
       <c r="AH12" s="7" t="s">
         <v>90</v>
       </c>
@@ -17229,7 +17317,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="13" spans="8:66">
       <c r="AH13" s="7" t="s">
         <v>65</v>
       </c>
@@ -17240,7 +17328,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="14" spans="8:66">
       <c r="AH14" s="7" t="s">
         <v>68</v>
       </c>
@@ -17251,7 +17339,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="15" spans="8:66">
       <c r="AH15" s="7" t="s">
         <v>73</v>
       </c>
@@ -17271,7 +17359,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="8:66" x14ac:dyDescent="0.15">
+    <row r="16" spans="8:66">
       <c r="AH16" s="7" t="s">
         <v>74</v>
       </c>
@@ -17285,7 +17373,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="17" spans="34:57">
       <c r="AH17" s="7" t="s">
         <v>75</v>
       </c>
@@ -17296,7 +17384,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="18" spans="34:57">
       <c r="AH18" s="55" t="s">
         <v>109</v>
       </c>
@@ -17311,7 +17399,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="19" spans="34:57">
       <c r="AH19" s="55" t="s">
         <v>115</v>
       </c>
@@ -17326,7 +17414,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="20" spans="34:57">
       <c r="AH20" s="60" t="s">
         <v>184</v>
       </c>
@@ -17337,7 +17425,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="21" spans="34:57">
       <c r="AH21" s="60" t="s">
         <v>185</v>
       </c>
@@ -17348,7 +17436,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="22" spans="34:57">
       <c r="AM22" s="7" t="s">
         <v>81</v>
       </c>
@@ -17356,12 +17444,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="23" spans="34:57">
       <c r="AM23" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="24" spans="34:57">
       <c r="AM24" s="7" t="s">
         <v>83</v>
       </c>
@@ -17372,7 +17460,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="25" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="25" spans="34:57">
       <c r="AM25" s="7" t="s">
         <v>84</v>
       </c>
@@ -17380,12 +17468,12 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="26" spans="34:57">
       <c r="AM26" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="27" spans="34:57">
       <c r="AM27" s="7" t="s">
         <v>86</v>
       </c>
@@ -17393,22 +17481,22 @@
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="28" spans="34:57">
       <c r="AT28" s="7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="29" spans="34:57">
       <c r="AT29" s="7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="30" spans="34:57">
       <c r="AT30" s="7" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="31" spans="34:57" x14ac:dyDescent="0.15">
+    <row r="31" spans="34:57">
       <c r="AT31" s="7" t="s">
         <v>220</v>
       </c>
@@ -17429,34 +17517,34 @@
       <selection activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:4">
       <c r="C3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:4">
       <c r="C4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:4">
       <c r="D5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:4">
       <c r="D6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:4">
       <c r="D7" t="s">
         <v>121</v>
       </c>
@@ -17476,14 +17564,14 @@
       <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:12">
       <c r="B2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:12">
       <c r="C3" t="s">
         <v>124</v>
       </c>
@@ -17491,7 +17579,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:12">
       <c r="D4" t="s">
         <v>125</v>
       </c>
@@ -17499,7 +17587,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:12">
       <c r="D5" t="s">
         <v>126</v>
       </c>
@@ -17507,7 +17595,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:12">
       <c r="D6" t="s">
         <v>127</v>
       </c>
@@ -17515,12 +17603,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:12">
       <c r="L7" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:12">
       <c r="C8" t="s">
         <v>128</v>
       </c>
@@ -17528,32 +17616,32 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:12">
       <c r="D9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:12">
       <c r="E10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:12">
       <c r="E11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:12">
       <c r="D12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:12">
       <c r="E13" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:12">
       <c r="E14" t="s">
         <v>134</v>
       </c>
@@ -17564,37 +17652,37 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:12">
       <c r="F15" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:12">
       <c r="C16" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:5">
       <c r="D17" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:5">
       <c r="E18" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="3:5">
       <c r="E19" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:5">
       <c r="E20" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="3:5">
       <c r="C21" t="s">
         <v>140</v>
       </c>
@@ -17605,7 +17693,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="3:5">
       <c r="D22" t="s">
         <v>143</v>
       </c>

</xml_diff>